<commit_message>
cleaned up small example; early days on production
</commit_message>
<xml_diff>
--- a/make-uniform/small-example/Example Dictionary.xlsx
+++ b/make-uniform/small-example/Example Dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="23">
   <si>
     <t>Survey</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Origin_Access_Mode</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -490,9 +493,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -671,19 +676,19 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,13 +699,13 @@
         <v>21</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>5</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,13 +716,13 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D13" t="s">
         <v>5</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,13 +733,13 @@
         <v>21</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
       </c>
       <c r="E14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -745,13 +750,13 @@
         <v>21</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
         <v>5</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -762,13 +767,13 @@
         <v>21</v>
       </c>
       <c r="C16">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -779,13 +784,13 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" t="s">
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -793,15 +798,49 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>18</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>19</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>